<commit_message>
adding s1/s2 and library sheets for Exp 29
</commit_message>
<xml_diff>
--- a/s1cDNASample/s1CDNASample_J.PLAGGENBERG_10.01.20.xlsx
+++ b/s1cDNASample/s1CDNASample_J.PLAGGENBERG_10.01.20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/s1cDNASample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94F2E835-376A-2547-B28F-39DF82243AA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487B8294-B310-5C47-A079-8C3DF5BF756E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15380" yWindow="460" windowWidth="15900" windowHeight="19860" xr2:uid="{F87C1414-C2A6-5040-991A-D5EBEA43D164}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>H.BROWN</t>
   </si>
   <si>
-    <t>10.01.2020</t>
-  </si>
-  <si>
     <t>J.PLAGGENBERG</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>random</t>
+  </si>
+  <si>
+    <t>10.01.20</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,25 +486,25 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -518,25 +518,25 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -550,25 +550,25 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -582,25 +582,25 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -614,25 +614,25 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -646,25 +646,25 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7" t="b">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -678,25 +678,25 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -710,25 +710,25 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -742,25 +742,25 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10">
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -774,25 +774,25 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -806,25 +806,25 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12">
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -838,25 +838,25 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13">
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I13" t="b">
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -870,25 +870,25 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14">
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I14" t="b">
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -902,25 +902,25 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15">
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -934,25 +934,25 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16">
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -966,25 +966,25 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17">
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -998,25 +998,25 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18">
         <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I18" t="b">
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -1030,25 +1030,25 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F19">
         <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I19" t="b">
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1062,25 +1062,25 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20">
         <v>19</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I20" t="b">
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1094,25 +1094,25 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F21">
         <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I21" t="b">
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1126,25 +1126,25 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F22">
         <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I22" t="b">
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -1158,25 +1158,25 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F23">
         <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I23" t="b">
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -1190,25 +1190,25 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F24">
         <v>23</v>
       </c>
       <c r="G24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I24" t="b">
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -1222,25 +1222,25 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F25">
         <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I25" t="b">
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1254,25 +1254,25 @@
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F26">
         <v>25</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -1286,25 +1286,25 @@
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F27">
         <v>26</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -1318,25 +1318,25 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F28">
         <v>27</v>
       </c>
       <c r="G28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I28" t="b">
         <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -1350,25 +1350,25 @@
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F29">
         <v>28</v>
       </c>
       <c r="G29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I29" t="b">
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>